<commit_message>
Updated rules and data 1/data2 to include zip
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
+++ b/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{467943DF-61E9-6D4E-B9FD-CB1FAE4604D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86CA77BD-8A89-B847-962F-514DEFE7ECD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="28320" windowHeight="16100" xr2:uid="{0CC8FC8D-9C2A-4C12-9288-CCE57E5F17EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>ImageFile</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>&gt;500</t>
+  </si>
+  <si>
+    <t>MicroplasticImages</t>
+  </si>
+  <si>
+    <t>ALGALITA_CW_3_above500_30.jpeg</t>
+  </si>
+  <si>
+    <t>B_DW_3_above500_96.jpeg</t>
+  </si>
+  <si>
+    <t>CC_CW_1_20-250_176.jpeg</t>
   </si>
 </sst>
 </file>
@@ -531,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179A76A1-E059-439E-BCF9-B9006BE755D0}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,8 +600,11 @@
       <c r="P1" t="s">
         <v>44</v>
       </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -632,8 +647,11 @@
       <c r="P2" t="s">
         <v>12</v>
       </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -679,8 +697,11 @@
       <c r="P3" t="s">
         <v>12</v>
       </c>
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -722,6 +743,9 @@
       </c>
       <c r="P4" t="s">
         <v>30</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a file for the zip code in microplastic_images, updated data1/data2
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
+++ b/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86CA77BD-8A89-B847-962F-514DEFE7ECD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB778C72-B026-AA48-B36E-98F2A66DBE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="28320" windowHeight="16100" xr2:uid="{0CC8FC8D-9C2A-4C12-9288-CCE57E5F17EB}"/>
   </bookViews>
@@ -185,13 +185,13 @@
     <t>MicroplasticImages</t>
   </si>
   <si>
-    <t>ALGALITA_CW_3_above500_30.jpeg</t>
-  </si>
-  <si>
-    <t>B_DW_3_above500_96.jpeg</t>
-  </si>
-  <si>
-    <t>CC_CW_1_20-250_176.jpeg</t>
+    <t>MicroplasticImages.zip/ALGALITA_CW_3_above500_30.jpeg</t>
+  </si>
+  <si>
+    <t>MicroplasticImages.zip/B_DW_3_above500_96.jpeg</t>
+  </si>
+  <si>
+    <t>MicroplasticImages.zip/CC_CW_1_20-250_176.jpeg</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added a zip file + updated rules/data1/data2
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
+++ b/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB778C72-B026-AA48-B36E-98F2A66DBE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20BA27BD-987C-D84B-B958-C420760DE405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="28320" windowHeight="16100" xr2:uid="{0CC8FC8D-9C2A-4C12-9288-CCE57E5F17EB}"/>
+    <workbookView xWindow="-36840" yWindow="-7440" windowWidth="28320" windowHeight="16100" xr2:uid="{0CC8FC8D-9C2A-4C12-9288-CCE57E5F17EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,13 +185,13 @@
     <t>MicroplasticImages</t>
   </si>
   <si>
-    <t>MicroplasticImages.zip/ALGALITA_CW_3_above500_30.jpeg</t>
-  </si>
-  <si>
-    <t>MicroplasticImages.zip/B_DW_3_above500_96.jpeg</t>
-  </si>
-  <si>
-    <t>MicroplasticImages.zip/CC_CW_1_20-250_176.jpeg</t>
+    <t>ALGALITA_CW_3_above500_30.jpeg</t>
+  </si>
+  <si>
+    <t>B_DW_3_above500_96.jpeg</t>
+  </si>
+  <si>
+    <t>CC_CW_1_20-250_176.jpeg</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates to image explorer; images showing as 3x10 rather than 2x15 (3 in each row, 10 each column)
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
+++ b/code/validator/www/microplastic_images/image_explorer_example_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20BA27BD-987C-D84B-B958-C420760DE405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A65251-4E9A-6449-9CD3-5FB7621ADEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36840" yWindow="-7440" windowWidth="28320" windowHeight="16100" xr2:uid="{0CC8FC8D-9C2A-4C12-9288-CCE57E5F17EB}"/>
   </bookViews>
@@ -546,7 +546,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>